<commit_message>
Moved all core functions to separate source file, and kept essential control flow in master script.
</commit_message>
<xml_diff>
--- a/example_output/Countyleveloutputs.xlsx
+++ b/example_output/Countyleveloutputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="2016Stock" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="88">
   <si>
     <t>County</t>
   </si>
@@ -660,131 +660,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:P3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>1465161</v>
+      </c>
+      <c r="C2">
+        <v>9862587</v>
+      </c>
+      <c r="D2">
+        <v>17338070</v>
+      </c>
+      <c r="E2">
+        <v>6229361</v>
+      </c>
+      <c r="F2">
+        <v>1323190</v>
+      </c>
+      <c r="G2">
+        <v>2192208</v>
+      </c>
+      <c r="H2">
+        <v>12946018</v>
+      </c>
+      <c r="I2">
+        <v>191623423</v>
+      </c>
+      <c r="J2">
+        <v>10090441</v>
+      </c>
+      <c r="K2">
+        <v>161205069</v>
+      </c>
+      <c r="L2">
+        <v>19802729</v>
+      </c>
+      <c r="M2">
+        <v>82597167</v>
+      </c>
+      <c r="N2">
+        <v>30598807</v>
+      </c>
+      <c r="O2">
+        <v>4764200</v>
+      </c>
+      <c r="P2">
+        <v>2246755</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3">
-        <v>1465161</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>9862587</v>
+        <v>14620.3633843799</v>
       </c>
       <c r="D3">
-        <v>17338070</v>
+        <v>1180671.4292727199</v>
       </c>
       <c r="E3">
-        <v>6229361</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1323190</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>2192208</v>
+        <v>4462.6712731799898</v>
       </c>
       <c r="H3">
-        <v>12946018</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>191623423</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>10090441</v>
+        <v>122764.4188306</v>
       </c>
       <c r="K3">
-        <v>161205069</v>
+        <v>109565.72417269</v>
       </c>
       <c r="L3">
-        <v>19802729</v>
+        <v>118016.708443271</v>
       </c>
       <c r="M3">
-        <v>82597167</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>30598807</v>
+        <v>1488.9890436369999</v>
       </c>
       <c r="O3">
-        <v>4764200</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>2246755</v>
+        <v>1317027.0593974199</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>14620.3633843799</v>
+        <v>3303221</v>
       </c>
       <c r="D4">
-        <v>1180671.4292727199</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -793,48 +838,48 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>4462.6712731799898</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>281228</v>
       </c>
       <c r="J4">
-        <v>122764.4188306</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>109565.72417269</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>118016.708443271</v>
+        <v>430971</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>1488.9890436369999</v>
+        <v>0</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>1317027.0593974199</v>
+        <v>66850</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>3303221</v>
+        <v>6146516</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1318448</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -849,895 +894,895 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>281228</v>
+        <v>8030712</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>19993299</v>
       </c>
       <c r="L5">
-        <v>430971</v>
+        <v>16145291</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>7984913</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
-        <v>66850</v>
+        <v>292910</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>6146516</v>
+        <v>411088</v>
       </c>
       <c r="D6">
-        <v>1318448</v>
+        <v>302551</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>12571</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>34055</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>84713</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>35834</v>
       </c>
       <c r="I6">
-        <v>8030712</v>
+        <v>317997</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>101134</v>
       </c>
       <c r="K6">
-        <v>19993299</v>
+        <v>517696</v>
       </c>
       <c r="L6">
-        <v>16145291</v>
+        <v>1643562</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>522983</v>
       </c>
       <c r="N6">
-        <v>7984913</v>
+        <v>245235</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>12571</v>
       </c>
       <c r="P6">
-        <v>292910</v>
+        <v>687060</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>411088</v>
+        <v>1115533</v>
       </c>
       <c r="D7">
-        <v>302551</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>12571</v>
+        <v>9361</v>
       </c>
       <c r="F7">
-        <v>34055</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>84713</v>
+        <v>171187</v>
       </c>
       <c r="H7">
-        <v>35834</v>
+        <v>48008</v>
       </c>
       <c r="I7">
-        <v>317997</v>
+        <v>766467</v>
       </c>
       <c r="J7">
-        <v>101134</v>
+        <v>153237</v>
       </c>
       <c r="K7">
-        <v>517696</v>
+        <v>613551</v>
       </c>
       <c r="L7">
-        <v>1643562</v>
+        <v>452378</v>
       </c>
       <c r="M7">
-        <v>522983</v>
+        <v>355162</v>
       </c>
       <c r="N7">
-        <v>245235</v>
+        <v>458305</v>
       </c>
       <c r="O7">
-        <v>12571</v>
+        <v>9361</v>
       </c>
       <c r="P7">
-        <v>687060</v>
+        <v>110104</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>180530</v>
       </c>
       <c r="C8">
-        <v>1115533</v>
+        <v>4233765</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>15247668</v>
       </c>
       <c r="E8">
-        <v>9361</v>
+        <v>2741413</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>702413</v>
       </c>
       <c r="G8">
-        <v>171187</v>
+        <v>1147624</v>
       </c>
       <c r="H8">
-        <v>48008</v>
+        <v>12178976</v>
       </c>
       <c r="I8">
-        <v>766467</v>
+        <v>39446587</v>
       </c>
       <c r="J8">
-        <v>153237</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>613551</v>
+        <v>58773557</v>
       </c>
       <c r="L8">
-        <v>452378</v>
+        <v>15281748</v>
       </c>
       <c r="M8">
-        <v>355162</v>
+        <v>61604267</v>
       </c>
       <c r="N8">
-        <v>458305</v>
+        <v>15504023</v>
       </c>
       <c r="O8">
-        <v>9361</v>
+        <v>2560883</v>
       </c>
       <c r="P8">
-        <v>110104</v>
+        <v>445917</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9">
-        <v>180530</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>4233765</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>15247668</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>2741413</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>702413</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>1147624</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>12178976</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>39446587</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>58773557</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>15281748</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>61604267</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>15504023</v>
+        <v>0</v>
       </c>
       <c r="O9">
-        <v>2560883</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>445917</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>511236</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>4337</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>153142</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>457230</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>488438</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>733352</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>4388406</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>1463435</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>6497465</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>3904603</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>2443786</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>4323659</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>153142</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>241916</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>2572815</v>
       </c>
       <c r="C11">
-        <v>511236</v>
+        <v>1134827</v>
       </c>
       <c r="D11">
-        <v>4337</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>153142</v>
+        <v>3997226</v>
       </c>
       <c r="F11">
-        <v>457230</v>
+        <v>4126425</v>
       </c>
       <c r="G11">
-        <v>488438</v>
+        <v>2368904</v>
       </c>
       <c r="H11">
-        <v>733352</v>
+        <v>9177086</v>
       </c>
       <c r="I11">
-        <v>4388406</v>
+        <v>252457017</v>
       </c>
       <c r="J11">
-        <v>1463435</v>
+        <v>4423971</v>
       </c>
       <c r="K11">
-        <v>6497465</v>
+        <v>67190950</v>
       </c>
       <c r="L11">
-        <v>3904603</v>
+        <v>15263772</v>
       </c>
       <c r="M11">
-        <v>2443786</v>
+        <v>22254665</v>
       </c>
       <c r="N11">
-        <v>4323659</v>
+        <v>25862777</v>
       </c>
       <c r="O11">
-        <v>153142</v>
+        <v>1424411</v>
       </c>
       <c r="P11">
-        <v>241916</v>
+        <v>1311638</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12">
-        <v>2572815</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>1134827</v>
+        <v>2360417</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>3997226</v>
+        <v>27969</v>
       </c>
       <c r="F12">
-        <v>4126425</v>
+        <v>111975</v>
       </c>
       <c r="G12">
-        <v>2368904</v>
+        <v>118349</v>
       </c>
       <c r="H12">
-        <v>9177086</v>
+        <v>106281</v>
       </c>
       <c r="I12">
-        <v>252457017</v>
+        <v>253197</v>
       </c>
       <c r="J12">
-        <v>4423971</v>
+        <v>156432</v>
       </c>
       <c r="K12">
-        <v>67190950</v>
+        <v>1224291</v>
       </c>
       <c r="L12">
-        <v>15263772</v>
+        <v>1018983</v>
       </c>
       <c r="M12">
-        <v>22254665</v>
+        <v>488673</v>
       </c>
       <c r="N12">
-        <v>25862777</v>
+        <v>541637</v>
       </c>
       <c r="O12">
-        <v>1424411</v>
+        <v>27969</v>
       </c>
       <c r="P12">
-        <v>1311638</v>
+        <v>69103</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>600000</v>
       </c>
       <c r="C13">
-        <v>2360417</v>
+        <v>1067424</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>28395</v>
       </c>
       <c r="E13">
-        <v>27969</v>
+        <v>610105</v>
       </c>
       <c r="F13">
-        <v>111975</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>118349</v>
+        <v>69924</v>
       </c>
       <c r="H13">
-        <v>106281</v>
+        <v>101776</v>
       </c>
       <c r="I13">
-        <v>253197</v>
+        <v>308129</v>
       </c>
       <c r="J13">
-        <v>156432</v>
+        <v>339133</v>
       </c>
       <c r="K13">
-        <v>1224291</v>
+        <v>1675722</v>
       </c>
       <c r="L13">
-        <v>1018983</v>
+        <v>313206</v>
       </c>
       <c r="M13">
-        <v>488673</v>
+        <v>485063</v>
       </c>
       <c r="N13">
-        <v>541637</v>
+        <v>423754</v>
       </c>
       <c r="O13">
-        <v>27969</v>
+        <v>10105</v>
       </c>
       <c r="P13">
-        <v>69103</v>
+        <v>83791</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>1067424</v>
+        <v>26254910.544939499</v>
       </c>
       <c r="D14">
-        <v>28395</v>
+        <v>33020.654586500001</v>
       </c>
       <c r="E14">
-        <v>610105</v>
+        <v>3139946.90282398</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14">
-        <v>69924</v>
+        <v>1337360.35647692</v>
       </c>
       <c r="H14">
-        <v>101776</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>308129</v>
+        <v>13281839.186333301</v>
       </c>
       <c r="J14">
-        <v>339133</v>
+        <v>1302077.9356639001</v>
       </c>
       <c r="K14">
-        <v>1675722</v>
+        <v>3745642.3368211202</v>
       </c>
       <c r="L14">
-        <v>313206</v>
+        <v>39409739.762456097</v>
       </c>
       <c r="M14">
-        <v>485063</v>
+        <v>11776035.7117553</v>
       </c>
       <c r="N14">
-        <v>423754</v>
+        <v>17491168.498776998</v>
       </c>
       <c r="O14">
-        <v>10105</v>
+        <v>3139946.90282398</v>
       </c>
       <c r="P14">
-        <v>83791</v>
+        <v>62744123.7945069</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15">
-        <v>26254910.544939499</v>
+        <v>584703</v>
       </c>
       <c r="D15">
-        <v>33020.654586500001</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>3139946.90282398</v>
+        <v>6778</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>185770</v>
       </c>
       <c r="G15">
-        <v>1337360.35647692</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>172983</v>
       </c>
       <c r="I15">
-        <v>13281839.186333301</v>
+        <v>398445</v>
       </c>
       <c r="J15">
-        <v>1302077.9356639001</v>
+        <v>472012</v>
       </c>
       <c r="K15">
-        <v>3745642.3368211202</v>
+        <v>1269862</v>
       </c>
       <c r="L15">
-        <v>39409739.762456097</v>
+        <v>776335</v>
       </c>
       <c r="M15">
-        <v>11776035.7117553</v>
+        <v>396050</v>
       </c>
       <c r="N15">
-        <v>17491168.498776998</v>
+        <v>299491</v>
       </c>
       <c r="O15">
-        <v>3139946.90282398</v>
+        <v>6778</v>
       </c>
       <c r="P15">
-        <v>62744123.7945069</v>
+        <v>21090</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1250000</v>
       </c>
       <c r="C16">
-        <v>584703</v>
+        <v>5624770</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>7685955</v>
       </c>
       <c r="E16">
-        <v>6778</v>
+        <v>2181045</v>
       </c>
       <c r="F16">
-        <v>185770</v>
+        <v>3141336</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>2485467</v>
       </c>
       <c r="H16">
-        <v>172983</v>
+        <v>4975110</v>
       </c>
       <c r="I16">
-        <v>398445</v>
+        <v>33728327</v>
       </c>
       <c r="J16">
-        <v>472012</v>
+        <v>4813527</v>
       </c>
       <c r="K16">
-        <v>1269862</v>
+        <v>61225853</v>
       </c>
       <c r="L16">
-        <v>776335</v>
+        <v>26541297</v>
       </c>
       <c r="M16">
-        <v>396050</v>
+        <v>12907238</v>
       </c>
       <c r="N16">
-        <v>299491</v>
+        <v>15065014</v>
       </c>
       <c r="O16">
-        <v>6778</v>
+        <v>931045</v>
       </c>
       <c r="P16">
-        <v>21090</v>
+        <v>19241789</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17">
-        <v>1250000</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>5624770</v>
+        <v>122483</v>
       </c>
       <c r="D17">
-        <v>7685955</v>
+        <v>524771</v>
       </c>
       <c r="E17">
-        <v>2181045</v>
+        <v>28214</v>
       </c>
       <c r="F17">
-        <v>3141336</v>
+        <v>539006</v>
       </c>
       <c r="G17">
-        <v>2485467</v>
+        <v>270564</v>
       </c>
       <c r="H17">
-        <v>4975110</v>
+        <v>320928</v>
       </c>
       <c r="I17">
-        <v>33728327</v>
+        <v>1616700</v>
       </c>
       <c r="J17">
-        <v>4813527</v>
+        <v>289887</v>
       </c>
       <c r="K17">
-        <v>61225853</v>
+        <v>3371059</v>
       </c>
       <c r="L17">
-        <v>26541297</v>
+        <v>1047300</v>
       </c>
       <c r="M17">
-        <v>12907238</v>
+        <v>1666566</v>
       </c>
       <c r="N17">
-        <v>15065014</v>
+        <v>1172072</v>
       </c>
       <c r="O17">
-        <v>931045</v>
+        <v>28214</v>
       </c>
       <c r="P17">
-        <v>19241789</v>
+        <v>206075</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>122483</v>
+        <v>731854</v>
       </c>
       <c r="D18">
-        <v>524771</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>28214</v>
+        <v>66748</v>
       </c>
       <c r="F18">
-        <v>539006</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>270564</v>
+        <v>168940</v>
       </c>
       <c r="H18">
-        <v>320928</v>
+        <v>225876</v>
       </c>
       <c r="I18">
-        <v>1616700</v>
+        <v>64483</v>
       </c>
       <c r="J18">
-        <v>289887</v>
+        <v>256499</v>
       </c>
       <c r="K18">
-        <v>3371059</v>
+        <v>1990746</v>
       </c>
       <c r="L18">
-        <v>1047300</v>
+        <v>379208</v>
       </c>
       <c r="M18">
-        <v>1666566</v>
+        <v>456319</v>
       </c>
       <c r="N18">
-        <v>1172072</v>
+        <v>1172069</v>
       </c>
       <c r="O18">
-        <v>28214</v>
+        <v>66748</v>
       </c>
       <c r="P18">
-        <v>206075</v>
+        <v>39369</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>731854</v>
+        <v>278252</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>66748</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19">
-        <v>168940</v>
+        <v>9931</v>
       </c>
       <c r="H19">
-        <v>225876</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>64483</v>
+        <v>9480</v>
       </c>
       <c r="J19">
-        <v>256499</v>
+        <v>0</v>
       </c>
       <c r="K19">
-        <v>1990746</v>
+        <v>1031993</v>
       </c>
       <c r="L19">
-        <v>379208</v>
+        <v>594106</v>
       </c>
       <c r="M19">
-        <v>456319</v>
+        <v>9778</v>
       </c>
       <c r="N19">
-        <v>1172069</v>
+        <v>3345</v>
       </c>
       <c r="O19">
-        <v>66748</v>
+        <v>0</v>
       </c>
       <c r="P19">
-        <v>39369</v>
+        <v>769</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>39462864</v>
       </c>
       <c r="C20">
-        <v>278252</v>
+        <v>13063964</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>383697918</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>67255175</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>9931</v>
+        <v>20181906</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>88231573</v>
       </c>
       <c r="I20">
-        <v>9480</v>
+        <v>910321974</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>67345447</v>
       </c>
       <c r="K20">
-        <v>1031993</v>
+        <v>1270861046</v>
       </c>
       <c r="L20">
-        <v>594106</v>
+        <v>156655312</v>
       </c>
       <c r="M20">
-        <v>9778</v>
+        <v>561184305</v>
       </c>
       <c r="N20">
-        <v>3345</v>
+        <v>240406215</v>
       </c>
       <c r="O20">
-        <v>0</v>
+        <v>27792311</v>
       </c>
       <c r="P20">
-        <v>769</v>
+        <v>7639047</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21">
-        <v>39462864</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>13063964</v>
+        <v>3193242</v>
       </c>
       <c r="D21">
-        <v>383697918</v>
+        <v>599728</v>
       </c>
       <c r="E21">
-        <v>67255175</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>404646</v>
       </c>
       <c r="G21">
-        <v>20181906</v>
+        <v>250461</v>
       </c>
       <c r="H21">
-        <v>88231573</v>
+        <v>350974</v>
       </c>
       <c r="I21">
-        <v>910321974</v>
+        <v>2636985</v>
       </c>
       <c r="J21">
-        <v>67345447</v>
+        <v>539477</v>
       </c>
       <c r="K21">
-        <v>1270861046</v>
+        <v>4232706</v>
       </c>
       <c r="L21">
-        <v>156655312</v>
+        <v>1949315</v>
       </c>
       <c r="M21">
-        <v>561184305</v>
+        <v>822890</v>
       </c>
       <c r="N21">
-        <v>240406215</v>
+        <v>160524</v>
       </c>
       <c r="O21">
-        <v>27792311</v>
+        <v>0</v>
       </c>
       <c r="P21">
-        <v>7639047</v>
+        <v>1033857</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>477460</v>
       </c>
       <c r="C22">
-        <v>3193242</v>
+        <v>30084796</v>
       </c>
       <c r="D22">
-        <v>599728</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>477460</v>
       </c>
       <c r="F22">
-        <v>404646</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>250461</v>
+        <v>0</v>
       </c>
       <c r="H22">
-        <v>350974</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>2636985</v>
+        <v>5501380</v>
       </c>
       <c r="J22">
-        <v>539477</v>
+        <v>0</v>
       </c>
       <c r="K22">
-        <v>4232706</v>
+        <v>3673204</v>
       </c>
       <c r="L22">
-        <v>1949315</v>
+        <v>823646</v>
       </c>
       <c r="M22">
-        <v>822890</v>
+        <v>6814603</v>
       </c>
       <c r="N22">
-        <v>160524</v>
+        <v>0</v>
       </c>
       <c r="O22">
         <v>0</v>
       </c>
       <c r="P22">
-        <v>1033857</v>
+        <v>181835</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23">
-        <v>477460</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>30084796</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>477460</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1749,19 +1794,19 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>5501380</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
-        <v>3673204</v>
+        <v>0</v>
       </c>
       <c r="L23">
-        <v>823646</v>
+        <v>0</v>
       </c>
       <c r="M23">
-        <v>6814603</v>
+        <v>0</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -1770,124 +1815,124 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <v>181835</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>3722051.91779191</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>2134056.23426593</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1022160.68949744</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>3144221.0491017201</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>32792547.0220914</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>11075514.1768496</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>5739377.8320759302</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>307509868.60225201</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>1555449.2085624</v>
       </c>
       <c r="N24">
-        <v>0</v>
+        <v>5316399.7005604301</v>
       </c>
       <c r="O24">
-        <v>0</v>
+        <v>2134056.23426593</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>36436893.251197703</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>990000</v>
       </c>
       <c r="C25">
-        <v>3722051.91779191</v>
+        <v>489723</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>2134056.23426593</v>
+        <v>990000</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25">
-        <v>1022160.68949744</v>
+        <v>0</v>
       </c>
       <c r="H25">
-        <v>3144221.0491017201</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>32792547.0220914</v>
+        <v>58448</v>
       </c>
       <c r="J25">
-        <v>11075514.1768496</v>
+        <v>0</v>
       </c>
       <c r="K25">
-        <v>5739377.8320759302</v>
+        <v>3113042</v>
       </c>
       <c r="L25">
-        <v>307509868.60225201</v>
+        <v>109663</v>
       </c>
       <c r="M25">
-        <v>1555449.2085624</v>
+        <v>98708</v>
       </c>
       <c r="N25">
-        <v>5316399.7005604301</v>
+        <v>0</v>
       </c>
       <c r="O25">
-        <v>2134056.23426593</v>
+        <v>0</v>
       </c>
       <c r="P25">
-        <v>36436893.251197703</v>
+        <v>17477</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B26">
-        <v>990000</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>489723</v>
+        <v>59348</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>990000</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1899,19 +1944,19 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>58448</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>2344</v>
       </c>
       <c r="K26">
-        <v>3113042</v>
+        <v>35772</v>
       </c>
       <c r="L26">
-        <v>109663</v>
+        <v>2612828</v>
       </c>
       <c r="M26">
-        <v>98708</v>
+        <v>0</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -1920,1762 +1965,1712 @@
         <v>0</v>
       </c>
       <c r="P26">
-        <v>17477</v>
+        <v>28396</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B27">
         <v>0</v>
       </c>
       <c r="C27">
-        <v>59348</v>
+        <v>1000</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>735385</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>3852</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>33435</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>156934</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>269394</v>
       </c>
       <c r="J27">
-        <v>2344</v>
+        <v>303450</v>
       </c>
       <c r="K27">
-        <v>35772</v>
+        <v>608871</v>
       </c>
       <c r="L27">
-        <v>2612828</v>
+        <v>459687</v>
       </c>
       <c r="M27">
-        <v>0</v>
+        <v>392916</v>
       </c>
       <c r="N27">
-        <v>0</v>
+        <v>73301</v>
       </c>
       <c r="O27">
-        <v>0</v>
+        <v>3852</v>
       </c>
       <c r="P27">
-        <v>28396</v>
+        <v>69156</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>2706</v>
       </c>
       <c r="C28">
-        <v>1000</v>
+        <v>9806523</v>
       </c>
       <c r="D28">
-        <v>735385</v>
+        <v>8345940</v>
       </c>
       <c r="E28">
-        <v>3852</v>
+        <v>281637</v>
       </c>
       <c r="F28">
-        <v>33435</v>
+        <v>377196</v>
       </c>
       <c r="G28">
-        <v>156934</v>
+        <v>735113</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>1171109</v>
       </c>
       <c r="I28">
-        <v>269394</v>
+        <v>8682073</v>
       </c>
       <c r="J28">
-        <v>303450</v>
+        <v>2611592</v>
       </c>
       <c r="K28">
-        <v>608871</v>
+        <v>11640846</v>
       </c>
       <c r="L28">
-        <v>459687</v>
+        <v>4913573</v>
       </c>
       <c r="M28">
-        <v>392916</v>
+        <v>6693876</v>
       </c>
       <c r="N28">
-        <v>73301</v>
+        <v>1351896</v>
       </c>
       <c r="O28">
-        <v>3852</v>
+        <v>278931</v>
       </c>
       <c r="P28">
-        <v>69156</v>
+        <v>129897</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B29">
-        <v>2706</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>9806523</v>
+        <v>4447793</v>
       </c>
       <c r="D29">
-        <v>8345940</v>
+        <v>3503357</v>
       </c>
       <c r="E29">
-        <v>281637</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>377196</v>
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>735113</v>
+        <v>0</v>
       </c>
       <c r="H29">
-        <v>1171109</v>
+        <v>0</v>
       </c>
       <c r="I29">
-        <v>8682073</v>
+        <v>12481813</v>
       </c>
       <c r="J29">
-        <v>2611592</v>
+        <v>1650271</v>
       </c>
       <c r="K29">
-        <v>11640846</v>
+        <v>3820673</v>
       </c>
       <c r="L29">
-        <v>4913573</v>
+        <v>237009</v>
       </c>
       <c r="M29">
-        <v>6693876</v>
+        <v>20734</v>
       </c>
       <c r="N29">
-        <v>1351896</v>
+        <v>0</v>
       </c>
       <c r="O29">
-        <v>278931</v>
+        <v>0</v>
       </c>
       <c r="P29">
-        <v>129897</v>
+        <v>595178</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30">
-        <v>4447793</v>
+        <v>819623</v>
       </c>
       <c r="D30">
-        <v>3503357</v>
+        <v>2478058</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>263614</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>262616</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>480758</v>
       </c>
       <c r="I30">
-        <v>12481813</v>
+        <v>2130424</v>
       </c>
       <c r="J30">
-        <v>1650271</v>
+        <v>651756</v>
       </c>
       <c r="K30">
-        <v>3820673</v>
+        <v>6047982</v>
       </c>
       <c r="L30">
-        <v>237009</v>
+        <v>4238538</v>
       </c>
       <c r="M30">
-        <v>20734</v>
+        <v>2104703</v>
       </c>
       <c r="N30">
-        <v>0</v>
+        <v>2048625</v>
       </c>
       <c r="O30">
         <v>0</v>
       </c>
       <c r="P30">
-        <v>595178</v>
+        <v>34634</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>1200000</v>
       </c>
       <c r="C31">
-        <v>819623</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>2478058</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>1200000</v>
       </c>
       <c r="F31">
-        <v>263614</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>262616</v>
+        <v>0</v>
       </c>
       <c r="H31">
-        <v>480758</v>
+        <v>0</v>
       </c>
       <c r="I31">
-        <v>2130424</v>
+        <v>0</v>
       </c>
       <c r="J31">
-        <v>651756</v>
+        <v>0</v>
       </c>
       <c r="K31">
-        <v>6047982</v>
+        <v>0</v>
       </c>
       <c r="L31">
-        <v>4238538</v>
+        <v>0</v>
       </c>
       <c r="M31">
-        <v>2104703</v>
+        <v>1689818</v>
       </c>
       <c r="N31">
-        <v>2048625</v>
+        <v>0</v>
       </c>
       <c r="O31">
         <v>0</v>
       </c>
       <c r="P31">
-        <v>34634</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32">
-        <v>1200000</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>530998</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>9510256</v>
       </c>
       <c r="E32">
-        <v>1200000</v>
+        <v>1053048</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>288048</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>1201269</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>3828059</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>21891545</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>2281922</v>
       </c>
       <c r="K32">
-        <v>0</v>
+        <v>14192272</v>
       </c>
       <c r="L32">
-        <v>0</v>
+        <v>6589355</v>
       </c>
       <c r="M32">
-        <v>1689818</v>
+        <v>14686567</v>
       </c>
       <c r="N32">
-        <v>0</v>
+        <v>13408948</v>
       </c>
       <c r="O32">
-        <v>0</v>
+        <v>1053048</v>
       </c>
       <c r="P32">
-        <v>0</v>
+        <v>186135</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33">
-        <v>530998</v>
+        <v>1386840</v>
       </c>
       <c r="D33">
-        <v>9510256</v>
+        <v>553232</v>
       </c>
       <c r="E33">
-        <v>1053048</v>
+        <v>0</v>
       </c>
       <c r="F33">
-        <v>288048</v>
+        <v>5725</v>
       </c>
       <c r="G33">
-        <v>1201269</v>
+        <v>0</v>
       </c>
       <c r="H33">
-        <v>3828059</v>
+        <v>6316</v>
       </c>
       <c r="I33">
-        <v>21891545</v>
+        <v>214695</v>
       </c>
       <c r="J33">
-        <v>2281922</v>
+        <v>55601</v>
       </c>
       <c r="K33">
-        <v>14192272</v>
+        <v>213355</v>
       </c>
       <c r="L33">
-        <v>6589355</v>
+        <v>2944481</v>
       </c>
       <c r="M33">
-        <v>14686567</v>
+        <v>33013</v>
       </c>
       <c r="N33">
-        <v>13408948</v>
+        <v>13015</v>
       </c>
       <c r="O33">
-        <v>1053048</v>
+        <v>0</v>
       </c>
       <c r="P33">
-        <v>186135</v>
+        <v>213992</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="C34">
-        <v>1386840</v>
+        <v>1068213</v>
       </c>
       <c r="D34">
-        <v>553232</v>
+        <v>87595350</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="F34">
-        <v>5725</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
       <c r="H34">
-        <v>6316</v>
+        <v>0</v>
       </c>
       <c r="I34">
-        <v>214695</v>
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>55601</v>
+        <v>0</v>
       </c>
       <c r="K34">
-        <v>213355</v>
+        <v>16735015</v>
       </c>
       <c r="L34">
-        <v>2944481</v>
+        <v>1380906</v>
       </c>
       <c r="M34">
-        <v>33013</v>
+        <v>0</v>
       </c>
       <c r="N34">
-        <v>13015</v>
+        <v>0</v>
       </c>
       <c r="O34">
         <v>0</v>
       </c>
       <c r="P34">
-        <v>213992</v>
+        <v>1692043</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B35">
-        <v>300000</v>
+        <v>3612693</v>
       </c>
       <c r="C35">
-        <v>1068213</v>
+        <v>4448819</v>
       </c>
       <c r="D35">
-        <v>87595350</v>
+        <v>65621</v>
       </c>
       <c r="E35">
-        <v>300000</v>
+        <v>7767583</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>3235769</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>3941915</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>15978543</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>103217213</v>
       </c>
       <c r="J35">
-        <v>0</v>
+        <v>7816075</v>
       </c>
       <c r="K35">
-        <v>16735015</v>
+        <v>104859517</v>
       </c>
       <c r="L35">
-        <v>1380906</v>
+        <v>23109804</v>
       </c>
       <c r="M35">
-        <v>0</v>
+        <v>84843483</v>
       </c>
       <c r="N35">
-        <v>0</v>
+        <v>28051216</v>
       </c>
       <c r="O35">
-        <v>0</v>
+        <v>4154890</v>
       </c>
       <c r="P35">
-        <v>1692043</v>
+        <v>1205652</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B36">
-        <v>3612693</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>4448819</v>
+        <v>6102</v>
       </c>
       <c r="D36">
-        <v>65621</v>
+        <v>23628</v>
       </c>
       <c r="E36">
-        <v>7767583</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>3235769</v>
+        <v>5822</v>
       </c>
       <c r="G36">
-        <v>3941915</v>
+        <v>6192</v>
       </c>
       <c r="H36">
-        <v>15978543</v>
+        <v>2098</v>
       </c>
       <c r="I36">
-        <v>103217213</v>
+        <v>217401</v>
       </c>
       <c r="J36">
-        <v>7816075</v>
+        <v>0</v>
       </c>
       <c r="K36">
-        <v>104859517</v>
+        <v>252194</v>
       </c>
       <c r="L36">
-        <v>23109804</v>
+        <v>52247</v>
       </c>
       <c r="M36">
-        <v>84843483</v>
+        <v>11575</v>
       </c>
       <c r="N36">
-        <v>28051216</v>
+        <v>15546</v>
       </c>
       <c r="O36">
-        <v>4154890</v>
+        <v>0</v>
       </c>
       <c r="P36">
-        <v>1205652</v>
+        <v>979</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>741223</v>
       </c>
       <c r="C37">
-        <v>6102</v>
+        <v>210338</v>
       </c>
       <c r="D37">
-        <v>23628</v>
+        <v>32017105</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>836993</v>
       </c>
       <c r="F37">
-        <v>5822</v>
+        <v>22981</v>
       </c>
       <c r="G37">
-        <v>6192</v>
+        <v>32467</v>
       </c>
       <c r="H37">
-        <v>2098</v>
+        <v>68645</v>
       </c>
       <c r="I37">
-        <v>217401</v>
+        <v>4206120</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>68421</v>
       </c>
       <c r="K37">
-        <v>252194</v>
+        <v>625707</v>
       </c>
       <c r="L37">
-        <v>52247</v>
+        <v>9608310</v>
       </c>
       <c r="M37">
-        <v>11575</v>
+        <v>236537</v>
       </c>
       <c r="N37">
-        <v>15546</v>
+        <v>272727</v>
       </c>
       <c r="O37">
-        <v>0</v>
+        <v>95770</v>
       </c>
       <c r="P37">
-        <v>979</v>
+        <v>3514982</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B38">
-        <v>741223</v>
+        <v>6046514</v>
       </c>
       <c r="C38">
-        <v>210338</v>
+        <v>93344163</v>
       </c>
       <c r="D38">
-        <v>32017105</v>
+        <v>218854094</v>
       </c>
       <c r="E38">
-        <v>836993</v>
+        <v>6046514</v>
       </c>
       <c r="F38">
-        <v>22981</v>
+        <v>6919507</v>
       </c>
       <c r="G38">
-        <v>32467</v>
+        <v>4895758</v>
       </c>
       <c r="H38">
-        <v>68645</v>
+        <v>6035093</v>
       </c>
       <c r="I38">
-        <v>4206120</v>
+        <v>115773512</v>
       </c>
       <c r="J38">
-        <v>68421</v>
+        <v>12345556</v>
       </c>
       <c r="K38">
-        <v>625707</v>
+        <v>239803912</v>
       </c>
       <c r="L38">
-        <v>9608310</v>
+        <v>62414688</v>
       </c>
       <c r="M38">
-        <v>236537</v>
+        <v>36859231</v>
       </c>
       <c r="N38">
-        <v>272727</v>
+        <v>0</v>
       </c>
       <c r="O38">
-        <v>95770</v>
+        <v>0</v>
       </c>
       <c r="P38">
-        <v>3514982</v>
+        <v>2360907</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B39">
-        <v>6046514</v>
+        <v>1384100</v>
       </c>
       <c r="C39">
-        <v>93344163</v>
+        <v>792582</v>
       </c>
       <c r="D39">
-        <v>218854094</v>
+        <v>56788203</v>
       </c>
       <c r="E39">
-        <v>6046514</v>
+        <v>4542456</v>
       </c>
       <c r="F39">
-        <v>6919507</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>4895758</v>
+        <v>0</v>
       </c>
       <c r="H39">
-        <v>6035093</v>
+        <v>4532011</v>
       </c>
       <c r="I39">
-        <v>115773512</v>
+        <v>25750573</v>
       </c>
       <c r="J39">
-        <v>12345556</v>
+        <v>24285830</v>
       </c>
       <c r="K39">
-        <v>239803912</v>
+        <v>163564097</v>
       </c>
       <c r="L39">
-        <v>62414688</v>
+        <v>32084324</v>
       </c>
       <c r="M39">
-        <v>36859231</v>
+        <v>92111747</v>
       </c>
       <c r="N39">
-        <v>0</v>
+        <v>25085547</v>
       </c>
       <c r="O39">
-        <v>0</v>
+        <v>3158356</v>
       </c>
       <c r="P39">
-        <v>2360907</v>
+        <v>1219048</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B40">
-        <v>1384100</v>
+        <v>1500000</v>
       </c>
       <c r="C40">
-        <v>792582</v>
+        <v>352843</v>
       </c>
       <c r="D40">
-        <v>56788203</v>
+        <v>4789285</v>
       </c>
       <c r="E40">
-        <v>4542456</v>
+        <v>1509081</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>2080</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>2990</v>
       </c>
       <c r="H40">
-        <v>4532011</v>
+        <v>36220</v>
       </c>
       <c r="I40">
-        <v>25750573</v>
+        <v>366625</v>
       </c>
       <c r="J40">
-        <v>24285830</v>
+        <v>65939</v>
       </c>
       <c r="K40">
-        <v>163564097</v>
+        <v>36017667</v>
       </c>
       <c r="L40">
-        <v>32084324</v>
+        <v>194390</v>
       </c>
       <c r="M40">
-        <v>92111747</v>
+        <v>179621</v>
       </c>
       <c r="N40">
-        <v>25085547</v>
+        <v>127000</v>
       </c>
       <c r="O40">
-        <v>3158356</v>
+        <v>9081</v>
       </c>
       <c r="P40">
-        <v>1219048</v>
+        <v>260890</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B41">
-        <v>1500000</v>
+        <v>0</v>
       </c>
       <c r="C41">
-        <v>352843</v>
+        <v>630949</v>
       </c>
       <c r="D41">
-        <v>4789285</v>
+        <v>6025116</v>
       </c>
       <c r="E41">
-        <v>1509081</v>
+        <v>47096</v>
       </c>
       <c r="F41">
-        <v>2080</v>
+        <v>283001</v>
       </c>
       <c r="G41">
-        <v>2990</v>
+        <v>289752</v>
       </c>
       <c r="H41">
-        <v>36220</v>
+        <v>639853</v>
       </c>
       <c r="I41">
-        <v>366625</v>
+        <v>1022876</v>
       </c>
       <c r="J41">
-        <v>65939</v>
+        <v>967210</v>
       </c>
       <c r="K41">
-        <v>36017667</v>
+        <v>8854428</v>
       </c>
       <c r="L41">
-        <v>194390</v>
+        <v>6041916</v>
       </c>
       <c r="M41">
-        <v>179621</v>
+        <v>1802100</v>
       </c>
       <c r="N41">
-        <v>127000</v>
+        <v>1645850</v>
       </c>
       <c r="O41">
-        <v>9081</v>
+        <v>47096</v>
       </c>
       <c r="P41">
-        <v>260890</v>
+        <v>660297</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>2104985</v>
       </c>
       <c r="C42">
-        <v>630949</v>
+        <v>141619</v>
       </c>
       <c r="D42">
-        <v>6025116</v>
+        <v>27024855</v>
       </c>
       <c r="E42">
-        <v>47096</v>
+        <v>2106295</v>
       </c>
       <c r="F42">
-        <v>283001</v>
+        <v>571616</v>
       </c>
       <c r="G42">
-        <v>289752</v>
+        <v>443614</v>
       </c>
       <c r="H42">
-        <v>639853</v>
+        <v>176097</v>
       </c>
       <c r="I42">
-        <v>1022876</v>
+        <v>27002370</v>
       </c>
       <c r="J42">
-        <v>967210</v>
+        <v>8797315</v>
       </c>
       <c r="K42">
-        <v>8854428</v>
+        <v>351021910</v>
       </c>
       <c r="L42">
-        <v>6041916</v>
+        <v>3106385</v>
       </c>
       <c r="M42">
-        <v>1802100</v>
+        <v>40596092</v>
       </c>
       <c r="N42">
-        <v>1645850</v>
+        <v>6022349</v>
       </c>
       <c r="O42">
-        <v>47096</v>
+        <v>1310</v>
       </c>
       <c r="P42">
-        <v>660297</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B43">
-        <v>2104985</v>
+        <v>8000000</v>
       </c>
       <c r="C43">
-        <v>141619</v>
+        <v>8387</v>
       </c>
       <c r="D43">
-        <v>27024855</v>
+        <v>16713736</v>
       </c>
       <c r="E43">
-        <v>2106295</v>
+        <v>8009851</v>
       </c>
       <c r="F43">
-        <v>571616</v>
+        <v>5763</v>
       </c>
       <c r="G43">
-        <v>443614</v>
+        <v>10972</v>
       </c>
       <c r="H43">
-        <v>176097</v>
+        <v>46859</v>
       </c>
       <c r="I43">
-        <v>27002370</v>
+        <v>48131</v>
       </c>
       <c r="J43">
-        <v>8797315</v>
+        <v>70084</v>
       </c>
       <c r="K43">
-        <v>351021910</v>
+        <v>2800098</v>
       </c>
       <c r="L43">
-        <v>3106385</v>
+        <v>4376710</v>
       </c>
       <c r="M43">
-        <v>40596092</v>
+        <v>108157</v>
       </c>
       <c r="N43">
-        <v>6022349</v>
+        <v>99919</v>
       </c>
       <c r="O43">
-        <v>1310</v>
+        <v>9851</v>
       </c>
       <c r="P43">
-        <v>0</v>
+        <v>190857</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B44">
-        <v>8000000</v>
+        <v>9072917.58611398</v>
       </c>
       <c r="C44">
-        <v>8387</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>16713736</v>
+        <v>106356880.338035</v>
       </c>
       <c r="E44">
-        <v>8009851</v>
+        <v>13481982.934739221</v>
       </c>
       <c r="F44">
-        <v>5763</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>10972</v>
+        <v>0</v>
       </c>
       <c r="H44">
-        <v>46859</v>
+        <v>5481841.9630460301</v>
       </c>
       <c r="I44">
-        <v>48131</v>
+        <v>118456837.32548299</v>
       </c>
       <c r="J44">
-        <v>70084</v>
+        <v>840449.38212700095</v>
       </c>
       <c r="K44">
-        <v>2800098</v>
+        <v>263508180.39073101</v>
       </c>
       <c r="L44">
-        <v>4376710</v>
+        <v>88322101.226025999</v>
       </c>
       <c r="M44">
-        <v>108157</v>
+        <v>100811747.391315</v>
       </c>
       <c r="N44">
-        <v>99919</v>
+        <v>0</v>
       </c>
       <c r="O44">
-        <v>9851</v>
+        <v>4409065.3486252399</v>
       </c>
       <c r="P44">
-        <v>190857</v>
+        <v>27044959.692522999</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B45">
-        <v>9072917.58611398</v>
+        <v>4187914</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>386329</v>
       </c>
       <c r="D45">
-        <v>106356880.338035</v>
+        <v>4949901</v>
       </c>
       <c r="E45">
-        <v>13481982.934739221</v>
+        <v>4318090</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>679285</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>493677</v>
       </c>
       <c r="H45">
-        <v>5481841.9630460301</v>
+        <v>1605115</v>
       </c>
       <c r="I45">
-        <v>118456837.32548299</v>
+        <v>5039480</v>
       </c>
       <c r="J45">
-        <v>840449.38212700095</v>
+        <v>1547811</v>
       </c>
       <c r="K45">
-        <v>263508180.39073101</v>
+        <v>8665803</v>
       </c>
       <c r="L45">
-        <v>88322101.226025999</v>
+        <v>3806947</v>
       </c>
       <c r="M45">
-        <v>100811747.391315</v>
+        <v>4261839</v>
       </c>
       <c r="N45">
-        <v>0</v>
+        <v>1723581</v>
       </c>
       <c r="O45">
-        <v>4409065.3486252399</v>
+        <v>130176</v>
       </c>
       <c r="P45">
-        <v>27044959.692522999</v>
+        <v>377693</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B46">
-        <v>4187914</v>
+        <v>20000</v>
       </c>
       <c r="C46">
-        <v>386329</v>
+        <v>2248773</v>
       </c>
       <c r="D46">
-        <v>4949901</v>
+        <v>719617</v>
       </c>
       <c r="E46">
-        <v>4318090</v>
+        <v>27102</v>
       </c>
       <c r="F46">
-        <v>679285</v>
+        <v>333797</v>
       </c>
       <c r="G46">
-        <v>493677</v>
+        <v>155650</v>
       </c>
       <c r="H46">
-        <v>1605115</v>
+        <v>601263</v>
       </c>
       <c r="I46">
-        <v>5039480</v>
+        <v>1323910</v>
       </c>
       <c r="J46">
-        <v>1547811</v>
+        <v>374924</v>
       </c>
       <c r="K46">
-        <v>8665803</v>
+        <v>5250472</v>
       </c>
       <c r="L46">
-        <v>3806947</v>
+        <v>17878251</v>
       </c>
       <c r="M46">
-        <v>4261839</v>
+        <v>1617074</v>
       </c>
       <c r="N46">
-        <v>1723581</v>
+        <v>2251453</v>
       </c>
       <c r="O46">
-        <v>130176</v>
+        <v>7102</v>
       </c>
       <c r="P46">
-        <v>377693</v>
+        <v>249447</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B47">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="C47">
-        <v>2248773</v>
+        <v>33739</v>
       </c>
       <c r="D47">
-        <v>719617</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>27102</v>
+        <v>0</v>
       </c>
       <c r="F47">
-        <v>333797</v>
+        <v>0</v>
       </c>
       <c r="G47">
-        <v>155650</v>
+        <v>45508</v>
       </c>
       <c r="H47">
-        <v>601263</v>
+        <v>0</v>
       </c>
       <c r="I47">
-        <v>1323910</v>
+        <v>1440</v>
       </c>
       <c r="J47">
-        <v>374924</v>
+        <v>17964</v>
       </c>
       <c r="K47">
-        <v>5250472</v>
+        <v>64140</v>
       </c>
       <c r="L47">
-        <v>17878251</v>
+        <v>45277</v>
       </c>
       <c r="M47">
-        <v>1617074</v>
+        <v>20220</v>
       </c>
       <c r="N47">
-        <v>2251453</v>
+        <v>44754</v>
       </c>
       <c r="O47">
-        <v>7102</v>
+        <v>0</v>
       </c>
       <c r="P47">
-        <v>249447</v>
+        <v>16468</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="C48">
-        <v>33739</v>
+        <v>35815</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>2587</v>
       </c>
       <c r="F48">
         <v>0</v>
       </c>
       <c r="G48">
-        <v>45508</v>
+        <v>684</v>
       </c>
       <c r="H48">
         <v>0</v>
       </c>
       <c r="I48">
-        <v>1440</v>
+        <v>17379</v>
       </c>
       <c r="J48">
-        <v>17964</v>
+        <v>0</v>
       </c>
       <c r="K48">
-        <v>64140</v>
+        <v>410779</v>
       </c>
       <c r="L48">
-        <v>45277</v>
+        <v>1669446</v>
       </c>
       <c r="M48">
-        <v>20220</v>
+        <v>9679</v>
       </c>
       <c r="N48">
-        <v>44754</v>
+        <v>0</v>
       </c>
       <c r="O48">
-        <v>0</v>
+        <v>2587</v>
       </c>
       <c r="P48">
-        <v>16468</v>
+        <v>84052</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>400000</v>
       </c>
       <c r="C49">
-        <v>35815</v>
+        <v>38920</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>6687561</v>
       </c>
       <c r="E49">
-        <v>2587</v>
+        <v>400000</v>
       </c>
       <c r="F49">
         <v>0</v>
       </c>
       <c r="G49">
-        <v>684</v>
+        <v>0</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>3526</v>
       </c>
       <c r="I49">
-        <v>17379</v>
+        <v>0</v>
       </c>
       <c r="J49">
         <v>0</v>
       </c>
       <c r="K49">
-        <v>410779</v>
+        <v>804728</v>
       </c>
       <c r="L49">
-        <v>1669446</v>
+        <v>512125</v>
       </c>
       <c r="M49">
-        <v>9679</v>
+        <v>0</v>
       </c>
       <c r="N49">
-        <v>0</v>
+        <v>1130</v>
       </c>
       <c r="O49">
-        <v>2587</v>
+        <v>0</v>
       </c>
       <c r="P49">
-        <v>84052</v>
+        <v>1862190</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B50">
-        <v>400000</v>
+        <v>3120000</v>
       </c>
       <c r="C50">
-        <v>38920</v>
+        <v>2831351</v>
       </c>
       <c r="D50">
-        <v>6687561</v>
+        <v>5760931</v>
       </c>
       <c r="E50">
-        <v>400000</v>
+        <v>4567519</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>774712</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>926838</v>
       </c>
       <c r="H50">
-        <v>3526</v>
+        <v>3446251</v>
       </c>
       <c r="I50">
-        <v>0</v>
+        <v>27731595</v>
       </c>
       <c r="J50">
-        <v>0</v>
+        <v>2283375</v>
       </c>
       <c r="K50">
-        <v>804728</v>
+        <v>21534011</v>
       </c>
       <c r="L50">
-        <v>512125</v>
+        <v>5740104</v>
       </c>
       <c r="M50">
-        <v>0</v>
+        <v>16819750</v>
       </c>
       <c r="N50">
-        <v>1130</v>
+        <v>5767286</v>
       </c>
       <c r="O50">
-        <v>0</v>
+        <v>1447519</v>
       </c>
       <c r="P50">
-        <v>1862190</v>
+        <v>805364</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B51">
-        <v>3120000</v>
+        <v>0</v>
       </c>
       <c r="C51">
-        <v>2831351</v>
+        <v>11342900</v>
       </c>
       <c r="D51">
-        <v>5760931</v>
+        <v>3161172</v>
       </c>
       <c r="E51">
-        <v>4567519</v>
+        <v>272202</v>
       </c>
       <c r="F51">
-        <v>774712</v>
+        <v>1452981</v>
       </c>
       <c r="G51">
-        <v>926838</v>
+        <v>1172935</v>
       </c>
       <c r="H51">
-        <v>3446251</v>
+        <v>3764877</v>
       </c>
       <c r="I51">
-        <v>27731595</v>
+        <v>53006171</v>
       </c>
       <c r="J51">
-        <v>2283375</v>
+        <v>1792069</v>
       </c>
       <c r="K51">
-        <v>21534011</v>
+        <v>19195181</v>
       </c>
       <c r="L51">
-        <v>5740104</v>
+        <v>4764428</v>
       </c>
       <c r="M51">
-        <v>16819750</v>
+        <v>14133652</v>
       </c>
       <c r="N51">
-        <v>5767286</v>
+        <v>7300759</v>
       </c>
       <c r="O51">
-        <v>1447519</v>
+        <v>272202</v>
       </c>
       <c r="P51">
-        <v>805364</v>
+        <v>171537</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
       <c r="C52">
-        <v>11342900</v>
+        <v>11263</v>
       </c>
       <c r="D52">
-        <v>3161172</v>
+        <v>572930</v>
       </c>
       <c r="E52">
-        <v>272202</v>
+        <v>169418</v>
       </c>
       <c r="F52">
-        <v>1452981</v>
+        <v>0</v>
       </c>
       <c r="G52">
-        <v>1172935</v>
+        <v>0</v>
       </c>
       <c r="H52">
-        <v>3764877</v>
+        <v>354560</v>
       </c>
       <c r="I52">
-        <v>53006171</v>
+        <v>5738953</v>
       </c>
       <c r="J52">
-        <v>1792069</v>
+        <v>282548</v>
       </c>
       <c r="K52">
-        <v>19195181</v>
+        <v>5179409</v>
       </c>
       <c r="L52">
-        <v>4764428</v>
+        <v>1761852</v>
       </c>
       <c r="M52">
-        <v>14133652</v>
+        <v>4309223</v>
       </c>
       <c r="N52">
-        <v>7300759</v>
+        <v>3948578</v>
       </c>
       <c r="O52">
-        <v>272202</v>
+        <v>169418</v>
       </c>
       <c r="P52">
-        <v>171537</v>
+        <v>137802</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="C53">
-        <v>11263</v>
+        <v>37907</v>
       </c>
       <c r="D53">
-        <v>572930</v>
+        <v>42572</v>
       </c>
       <c r="E53">
-        <v>169418</v>
+        <v>47057</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>126182</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>43955</v>
       </c>
       <c r="H53">
-        <v>354560</v>
+        <v>137275</v>
       </c>
       <c r="I53">
-        <v>5738953</v>
+        <v>388714</v>
       </c>
       <c r="J53">
-        <v>282548</v>
+        <v>46284</v>
       </c>
       <c r="K53">
-        <v>5179409</v>
+        <v>321866</v>
       </c>
       <c r="L53">
-        <v>1761852</v>
+        <v>23950525</v>
       </c>
       <c r="M53">
-        <v>4309223</v>
+        <v>585016</v>
       </c>
       <c r="N53">
-        <v>3948578</v>
+        <v>865870</v>
       </c>
       <c r="O53">
-        <v>169418</v>
+        <v>47057</v>
       </c>
       <c r="P53">
-        <v>137802</v>
+        <v>137502</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
       <c r="C54">
-        <v>37907</v>
+        <v>150180</v>
       </c>
       <c r="D54">
-        <v>42572</v>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>47057</v>
+        <v>0</v>
       </c>
       <c r="F54">
-        <v>126182</v>
+        <v>0</v>
       </c>
       <c r="G54">
-        <v>43955</v>
+        <v>0</v>
       </c>
       <c r="H54">
-        <v>137275</v>
+        <v>0</v>
       </c>
       <c r="I54">
-        <v>388714</v>
+        <v>22380</v>
       </c>
       <c r="J54">
-        <v>46284</v>
+        <v>15532</v>
       </c>
       <c r="K54">
-        <v>321866</v>
+        <v>100763</v>
       </c>
       <c r="L54">
-        <v>23950525</v>
+        <v>428582</v>
       </c>
       <c r="M54">
-        <v>585016</v>
+        <v>15845</v>
       </c>
       <c r="N54">
-        <v>865870</v>
+        <v>0</v>
       </c>
       <c r="O54">
-        <v>47057</v>
+        <v>0</v>
       </c>
       <c r="P54">
-        <v>137502</v>
+        <v>8064</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55">
-        <v>150180</v>
+        <v>684434</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>3133054</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>465072</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>980515</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>982396</v>
       </c>
       <c r="H55">
-        <v>0</v>
+        <v>3631832</v>
       </c>
       <c r="I55">
-        <v>22380</v>
+        <v>25980136</v>
       </c>
       <c r="J55">
-        <v>15532</v>
+        <v>1341276</v>
       </c>
       <c r="K55">
-        <v>100763</v>
+        <v>15377584</v>
       </c>
       <c r="L55">
-        <v>428582</v>
+        <v>10196900</v>
       </c>
       <c r="M55">
-        <v>15845</v>
+        <v>8089852</v>
       </c>
       <c r="N55">
-        <v>0</v>
+        <v>3981647</v>
       </c>
       <c r="O55">
-        <v>0</v>
+        <v>465072</v>
       </c>
       <c r="P55">
-        <v>8064</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
       <c r="C56">
-        <v>684434</v>
+        <v>4525698</v>
       </c>
       <c r="D56">
-        <v>3133054</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>465072</v>
+        <v>0</v>
       </c>
       <c r="F56">
-        <v>980515</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>982396</v>
+        <v>0</v>
       </c>
       <c r="H56">
-        <v>3631832</v>
+        <v>0</v>
       </c>
       <c r="I56">
-        <v>25980136</v>
+        <v>781499</v>
       </c>
       <c r="J56">
-        <v>1341276</v>
+        <v>161689</v>
       </c>
       <c r="K56">
-        <v>15377584</v>
+        <v>1343955</v>
       </c>
       <c r="L56">
-        <v>10196900</v>
+        <v>3492441</v>
       </c>
       <c r="M56">
-        <v>8089852</v>
+        <v>0</v>
       </c>
       <c r="N56">
-        <v>3981647</v>
+        <v>0</v>
       </c>
       <c r="O56">
-        <v>465072</v>
+        <v>0</v>
       </c>
       <c r="P56">
-        <v>0</v>
+        <v>2736588</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>3849766</v>
       </c>
       <c r="C57">
-        <v>4525698</v>
+        <v>37449</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>49987077</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>3864513</v>
       </c>
       <c r="F57">
         <v>0</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1392</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>121651</v>
       </c>
       <c r="I57">
-        <v>781499</v>
+        <v>7057</v>
       </c>
       <c r="J57">
-        <v>161689</v>
+        <v>73925</v>
       </c>
       <c r="K57">
-        <v>1343955</v>
+        <v>9252192</v>
       </c>
       <c r="L57">
-        <v>3492441</v>
+        <v>1976244</v>
       </c>
       <c r="M57">
-        <v>0</v>
+        <v>78549</v>
       </c>
       <c r="N57">
         <v>0</v>
       </c>
       <c r="O57">
-        <v>0</v>
+        <v>14747</v>
       </c>
       <c r="P57">
-        <v>2736588</v>
+        <v>660968</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B58">
-        <v>3849766</v>
+        <v>100000</v>
       </c>
       <c r="C58">
-        <v>37449</v>
+        <v>72898</v>
       </c>
       <c r="D58">
-        <v>49987077</v>
+        <v>1976044</v>
       </c>
       <c r="E58">
-        <v>3864513</v>
+        <v>134378</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>190333</v>
       </c>
       <c r="G58">
-        <v>1392</v>
+        <v>221152</v>
       </c>
       <c r="H58">
-        <v>121651</v>
+        <v>302113</v>
       </c>
       <c r="I58">
-        <v>7057</v>
+        <v>15417136</v>
       </c>
       <c r="J58">
-        <v>73925</v>
+        <v>452626</v>
       </c>
       <c r="K58">
-        <v>9252192</v>
+        <v>12530232</v>
       </c>
       <c r="L58">
-        <v>1976244</v>
+        <v>1052122</v>
       </c>
       <c r="M58">
-        <v>78549</v>
+        <v>2629787</v>
       </c>
       <c r="N58">
-        <v>0</v>
+        <v>1472588</v>
       </c>
       <c r="O58">
-        <v>14747</v>
+        <v>34378</v>
       </c>
       <c r="P58">
-        <v>660968</v>
+        <v>327343</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B59">
-        <v>100000</v>
+        <v>150000</v>
       </c>
       <c r="C59">
-        <v>72898</v>
+        <v>355580</v>
       </c>
       <c r="D59">
-        <v>1976044</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>134378</v>
+        <v>150000</v>
       </c>
       <c r="F59">
-        <v>190333</v>
+        <v>0</v>
       </c>
       <c r="G59">
-        <v>221152</v>
+        <v>147733</v>
       </c>
       <c r="H59">
-        <v>302113</v>
+        <v>292961</v>
       </c>
       <c r="I59">
-        <v>15417136</v>
+        <v>1649744</v>
       </c>
       <c r="J59">
-        <v>452626</v>
+        <v>216260</v>
       </c>
       <c r="K59">
-        <v>12530232</v>
+        <v>1553721</v>
       </c>
       <c r="L59">
-        <v>1052122</v>
+        <v>2249320</v>
       </c>
       <c r="M59">
-        <v>2629787</v>
+        <v>1897523</v>
       </c>
       <c r="N59">
-        <v>1472588</v>
+        <v>1735460</v>
       </c>
       <c r="O59">
-        <v>34378</v>
+        <v>0</v>
       </c>
       <c r="P59">
-        <v>327343</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>75</v>
-      </c>
-      <c r="B60">
-        <v>150000</v>
-      </c>
-      <c r="C60">
-        <v>355580</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
-        <v>150000</v>
-      </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
-      <c r="G60">
-        <v>147733</v>
-      </c>
-      <c r="H60">
-        <v>292961</v>
-      </c>
-      <c r="I60">
-        <v>1649744</v>
-      </c>
-      <c r="J60">
-        <v>216260</v>
-      </c>
-      <c r="K60">
-        <v>1553721</v>
-      </c>
-      <c r="L60">
-        <v>2249320</v>
-      </c>
-      <c r="M60">
-        <v>1897523</v>
-      </c>
-      <c r="N60">
-        <v>1735460</v>
-      </c>
-      <c r="O60">
-        <v>0</v>
-      </c>
-      <c r="P60">
         <v>138336</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>76</v>
       </c>
-      <c r="B62">
+      <c r="B61">
         <v>92791648.586113974</v>
       </c>
-      <c r="C62">
+      <c r="C61">
         <v>255161359.82611579</v>
       </c>
-      <c r="D62">
+      <c r="D61">
         <v>1086332493.4218941</v>
       </c>
-      <c r="E62">
+      <c r="E61">
         <v>151664898.07182914</v>
       </c>
-      <c r="F62">
+      <c r="F61">
         <v>27578408</v>
       </c>
-      <c r="G62">
+      <c r="G61">
         <v>48544111.717247538</v>
       </c>
-      <c r="H62">
+      <c r="H61">
         <v>185493923.01214775</v>
       </c>
-      <c r="I62">
+      <c r="I61">
         <v>2077120967.5339077</v>
       </c>
-      <c r="J62">
+      <c r="J61">
         <v>174365086.9134711</v>
       </c>
-      <c r="K62">
+      <c r="K61">
         <v>3004243029.2838006</v>
       </c>
-      <c r="L62">
+      <c r="L61">
         <v>942382866.29917741</v>
       </c>
-      <c r="M62">
+      <c r="M61">
         <v>1206089634.3116326</v>
       </c>
-      <c r="N62">
+      <c r="N61">
         <v>474339942.18838108</v>
       </c>
-      <c r="O62">
+      <c r="O61">
         <v>58873249.485715158</v>
       </c>
-      <c r="P62">
+      <c r="P61">
         <v>181556752.79762504</v>
       </c>
     </row>
   </sheetData>
   <sortState columnSort="1" ref="B1:P62">
-    <sortCondition ref="B2:P2"/>
+    <sortCondition ref="B1:P1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16677,7 +16672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:O60"/>
     </sheetView>
   </sheetViews>

</xml_diff>